<commit_message>
Update Edit text Suite
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Arctick\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6F94DF-7116-4465-B3D0-518535BDB3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B3912-F624-47D4-8CC7-1171B08D34F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Onboarding" sheetId="11" r:id="rId1"/>
@@ -3383,12 +3383,6 @@
     <t>Hebrew</t>
   </si>
   <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t>Turkish</t>
-  </si>
-  <si>
     <t>Space</t>
   </si>
   <si>
@@ -3435,6 +3429,12 @@
   </si>
   <si>
     <t>Bespoke</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -3584,7 +3584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3673,6 +3673,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3990,7 +3991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEEA25A-B9EE-4434-8603-4CD75E6C0C65}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+    <sheetView topLeftCell="H13" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
@@ -4078,13 +4079,13 @@
     </row>
     <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>1055</v>
@@ -4099,7 +4100,7 @@
         <v>1058</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="M2" s="31" t="s">
         <v>1059</v>
@@ -4114,13 +4115,13 @@
         <v>1072</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R2" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T2" s="31">
         <v>100</v>
@@ -4128,13 +4129,13 @@
     </row>
     <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="H3" s="31" t="s">
         <v>1055</v>
@@ -4149,7 +4150,7 @@
         <v>1058</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>1059</v>
@@ -4164,13 +4165,13 @@
         <v>1072</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R3" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S3" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T3" s="31">
         <v>0</v>
@@ -4178,13 +4179,13 @@
     </row>
     <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="H4" s="31" t="s">
         <v>1055</v>
@@ -4199,7 +4200,7 @@
         <v>1058</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="M4" s="31" t="s">
         <v>1059</v>
@@ -4214,13 +4215,13 @@
         <v>1072</v>
       </c>
       <c r="Q4" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R4" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T4" s="31">
         <v>100</v>
@@ -4228,13 +4229,13 @@
     </row>
     <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="H5" s="31" t="s">
         <v>1055</v>
@@ -4249,7 +4250,7 @@
         <v>1058</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>1059</v>
@@ -4264,13 +4265,13 @@
         <v>1072</v>
       </c>
       <c r="Q5" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R5" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T5" s="31">
         <v>0</v>
@@ -4278,13 +4279,13 @@
     </row>
     <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="H6" s="31" t="s">
         <v>1055</v>
@@ -4299,7 +4300,7 @@
         <v>1058</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="M6" s="31" t="s">
         <v>1059</v>
@@ -4314,13 +4315,13 @@
         <v>1072</v>
       </c>
       <c r="Q6" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R6" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S6" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T6" s="31">
         <v>100</v>
@@ -4328,13 +4329,13 @@
     </row>
     <row r="7" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="H7" s="31" t="s">
         <v>1055</v>
@@ -4349,7 +4350,7 @@
         <v>1058</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>1059</v>
@@ -4364,13 +4365,13 @@
         <v>1072</v>
       </c>
       <c r="Q7" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R7" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S7" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T7" s="31">
         <v>0</v>
@@ -4378,13 +4379,13 @@
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="H8" s="31" t="s">
         <v>1055</v>
@@ -4399,7 +4400,7 @@
         <v>1058</v>
       </c>
       <c r="L8" s="31" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="M8" s="31" t="s">
         <v>1059</v>
@@ -4414,13 +4415,13 @@
         <v>1072</v>
       </c>
       <c r="Q8" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R8" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S8" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T8" s="31">
         <v>100</v>
@@ -4428,13 +4429,13 @@
     </row>
     <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="H9" s="31" t="s">
         <v>1055</v>
@@ -4449,7 +4450,7 @@
         <v>1058</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="M9" s="31" t="s">
         <v>1059</v>
@@ -4464,13 +4465,13 @@
         <v>1072</v>
       </c>
       <c r="Q9" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R9" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T9" s="31">
         <v>0</v>
@@ -4478,13 +4479,13 @@
     </row>
     <row r="10" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>1055</v>
@@ -4499,7 +4500,7 @@
         <v>1058</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="M10" s="31" t="s">
         <v>1059</v>
@@ -4514,13 +4515,13 @@
         <v>1072</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R10" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S10" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T10" s="31">
         <v>100</v>
@@ -4528,13 +4529,13 @@
     </row>
     <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="H11" s="31" t="s">
         <v>1055</v>
@@ -4549,7 +4550,7 @@
         <v>1058</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="M11" s="31" t="s">
         <v>1059</v>
@@ -4564,13 +4565,13 @@
         <v>1072</v>
       </c>
       <c r="Q11" s="34" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R11" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S11" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T11" s="31">
         <v>0</v>
@@ -4578,13 +4579,13 @@
     </row>
     <row r="12" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="H12" s="31" t="s">
         <v>1055</v>
@@ -4599,7 +4600,7 @@
         <v>1058</v>
       </c>
       <c r="L12" s="31" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="M12" s="31" t="s">
         <v>1059</v>
@@ -4614,13 +4615,13 @@
         <v>1072</v>
       </c>
       <c r="Q12" s="34" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="R12" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S12" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T12" s="31">
         <v>100</v>
@@ -4628,13 +4629,13 @@
     </row>
     <row r="13" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>1055</v>
@@ -4649,7 +4650,7 @@
         <v>1058</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="M13" s="31" t="s">
         <v>1059</v>
@@ -4664,13 +4665,13 @@
         <v>1072</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="R13" s="31" t="s">
         <v>1074</v>
       </c>
       <c r="S13" s="31" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="T13" s="31">
         <v>0</v>
@@ -7986,8 +7987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2071D1-0EBD-4D0F-8C4E-9114D9657196}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8001,83 +8002,83 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1100</v>
+      <c r="A2" s="36" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1115</v>
+        <v>1131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Text Bespoke Del 2
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Arctick\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B3912-F624-47D4-8CC7-1171B08D34F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8700E994-352E-4343-A793-1EF0FE165D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="2" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Onboarding" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2820" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2657" uniqueCount="1120">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -3254,87 +3254,12 @@
     <t>Coverimage</t>
   </si>
   <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\LogoLayout\\logo2.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\LogoLayout\\coverimage3.jpg</t>
-  </si>
-  <si>
     <t>Admin Fee</t>
   </si>
   <si>
     <t>Theme 2</t>
   </si>
   <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\1.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\2.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\3.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\4.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\5.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\6.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\7.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\8.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\9.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\10.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\11.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\12.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\13.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\14.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\15.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\16.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\17.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\18.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\19.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\20.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\21.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\22.png</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Arctick\\Images\\Category\\23.png</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
@@ -3383,51 +3308,12 @@
     <t>Hebrew</t>
   </si>
   <si>
-    <t>Space</t>
-  </si>
-  <si>
     <t>SGD</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>0220BP100COMM1</t>
-  </si>
-  <si>
-    <t>0220BP0COMM2</t>
-  </si>
-  <si>
-    <t>0220BP100COMM3</t>
-  </si>
-  <si>
-    <t>0220BP0COMM4</t>
-  </si>
-  <si>
-    <t>0220BP100COMM5</t>
-  </si>
-  <si>
-    <t>0220BP0COMM6</t>
-  </si>
-  <si>
-    <t>0220BP100COMM7</t>
-  </si>
-  <si>
-    <t>0220BP0COMM8</t>
-  </si>
-  <si>
-    <t>0220BP100COMM9</t>
-  </si>
-  <si>
-    <t>0220BP0COMM10</t>
-  </si>
-  <si>
-    <t>0220ST0COMM</t>
-  </si>
-  <si>
-    <t>0220ST100COMM</t>
-  </si>
-  <si>
     <t>Bespoke</t>
   </si>
   <si>
@@ -3435,6 +3321,84 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\LogoLayout\\logo2.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\LogoLayout\\coverimage3.jpg</t>
+  </si>
+  <si>
+    <t>0319BPDEL2</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\1.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\2.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\3.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\4.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\5.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\6.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\7.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\8.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\9.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\10.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\11.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\12.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\13.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\14.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\15.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\16.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\17.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\18.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\19.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\20.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\21.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\22.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\Arctick\\Images\\Category\\23.png</t>
   </si>
 </sst>
 </file>
@@ -3989,27 +3953,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEEA25A-B9EE-4434-8603-4CD75E6C0C65}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.7109375" style="31" customWidth="1"/>
-    <col min="3" max="5" width="17.140625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="30" style="31" customWidth="1"/>
+    <col min="4" max="5" width="17.140625" style="31" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="31" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="31" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" style="31" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" style="31" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="31" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="31" customWidth="1"/>
     <col min="13" max="13" width="12" style="31" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" style="31" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" style="31" customWidth="1"/>
+    <col min="15" max="15" width="52.140625" style="31" customWidth="1"/>
+    <col min="16" max="16" width="70.42578125" style="31" customWidth="1"/>
     <col min="17" max="17" width="23.85546875" style="31" customWidth="1"/>
     <col min="18" max="19" width="11.5703125" style="31" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="31"/>
@@ -4074,18 +4039,18 @@
         <v>1053</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>1116</v>
+        <v>1090</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>1064</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>1117</v>
+        <v>1096</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>1055</v>
@@ -4100,7 +4065,7 @@
         <v>1058</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>1117</v>
+        <v>1096</v>
       </c>
       <c r="M2" s="31" t="s">
         <v>1059</v>
@@ -4109,587 +4074,88 @@
         <v>1060</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>1071</v>
+        <v>1094</v>
       </c>
       <c r="P2" s="33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>1091</v>
+      </c>
+      <c r="R2" s="31" t="s">
         <v>1072</v>
       </c>
-      <c r="Q2" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R2" s="31" t="s">
-        <v>1074</v>
-      </c>
       <c r="S2" s="31" t="s">
-        <v>1115</v>
+        <v>1089</v>
       </c>
       <c r="T2" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>1118</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>1118</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N3" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P3" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q3" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R3" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S3" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T3" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>1119</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>1119</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N4" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P4" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q4" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R4" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S4" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T4" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>1120</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>1120</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P5" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q5" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R5" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S5" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T5" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>1121</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L6" s="31" t="s">
-        <v>1121</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O6" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P6" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R6" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S6" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T6" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>1122</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J7" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K7" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L7" s="31" t="s">
-        <v>1122</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P7" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R7" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S7" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T7" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>1123</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>1123</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N8" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O8" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P8" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q8" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R8" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T8" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>1124</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>1124</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O9" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P9" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q9" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R9" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S9" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T9" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>1125</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K10" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>1125</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R10" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S10" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T10" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K11" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>1126</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N11" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O11" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P11" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>1129</v>
-      </c>
-      <c r="R11" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S11" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T11" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>1128</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I12" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L12" s="31" t="s">
-        <v>1127</v>
-      </c>
-      <c r="M12" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N12" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O12" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P12" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q12" s="34" t="s">
-        <v>1114</v>
-      </c>
-      <c r="R12" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S12" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T12" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K13" s="32" t="s">
-        <v>1058</v>
-      </c>
-      <c r="L13" s="31" t="s">
-        <v>1128</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N13" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O13" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="P13" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="Q13" s="34" t="s">
-        <v>1114</v>
-      </c>
-      <c r="R13" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>1115</v>
-      </c>
-      <c r="T13" s="31">
-        <v>0</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K4" s="32"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K5" s="32"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K6" s="32"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K7" s="32"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="34"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K8" s="32"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="34"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K9" s="32"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="34"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K10" s="32"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="34"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{BB45C7F2-3FEA-4FD4-91BF-7C08B068B1D9}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{C29D5C53-FC26-4924-AD0E-D65FD2504398}"/>
-    <hyperlink ref="N4:N13" r:id="rId3" display="arcadierteam@gmail.com" xr:uid="{A323ECED-99C2-4680-9F28-D97EFEE86C98}"/>
+    <hyperlink ref="N2:N5" r:id="rId1" display="arcadierteam@gmail.com" xr:uid="{A323ECED-99C2-4680-9F28-D97EFEE86C98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <ignoredErrors>
-    <ignoredError sqref="K2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7987,7 +7453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2071D1-0EBD-4D0F-8C4E-9114D9657196}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -7998,87 +7464,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>1099</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>1130</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1100</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1101</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1102</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1103</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1104</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1105</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1106</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1107</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1108</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1109</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1110</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1111</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1112</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1113</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1131</v>
+        <v>1093</v>
       </c>
     </row>
   </sheetData>
@@ -8091,8 +7557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D89469-70B5-42D0-9A59-1DD22F5E00A8}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C85" activeCellId="1" sqref="B80 C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8125,7 +7591,7 @@
         <v>720</v>
       </c>
       <c r="C2" t="s">
-        <v>1075</v>
+        <v>1097</v>
       </c>
       <c r="D2" t="s">
         <v>723</v>
@@ -8139,7 +7605,7 @@
         <v>720</v>
       </c>
       <c r="C3" t="s">
-        <v>1076</v>
+        <v>1098</v>
       </c>
       <c r="D3" t="s">
         <v>724</v>
@@ -8153,7 +7619,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>1076</v>
+        <v>1098</v>
       </c>
       <c r="D4" t="s">
         <v>725</v>
@@ -8167,7 +7633,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>1076</v>
+        <v>1098</v>
       </c>
       <c r="D5" t="s">
         <v>726</v>
@@ -8181,7 +7647,7 @@
         <v>720</v>
       </c>
       <c r="C6" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="D6" t="s">
         <v>727</v>
@@ -8195,7 +7661,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="D7" t="s">
         <v>728</v>
@@ -8209,7 +7675,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="D8" t="s">
         <v>729</v>
@@ -8223,7 +7689,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="D9" t="s">
         <v>730</v>
@@ -8237,7 +7703,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="D10" t="s">
         <v>731</v>
@@ -8251,7 +7717,7 @@
         <v>720</v>
       </c>
       <c r="C11" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D11" t="s">
         <v>732</v>
@@ -8265,7 +7731,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D12" t="s">
         <v>733</v>
@@ -8279,7 +7745,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D13" t="s">
         <v>734</v>
@@ -8293,7 +7759,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D14" t="s">
         <v>735</v>
@@ -8307,7 +7773,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D15" t="s">
         <v>736</v>
@@ -8321,7 +7787,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D16" t="s">
         <v>737</v>
@@ -8335,7 +7801,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D17" t="s">
         <v>738</v>
@@ -8349,7 +7815,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D18" t="s">
         <v>739</v>
@@ -8363,7 +7829,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D19" t="s">
         <v>740</v>
@@ -8377,7 +7843,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D20" t="s">
         <v>741</v>
@@ -8391,7 +7857,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D21" t="s">
         <v>742</v>
@@ -8405,7 +7871,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D22" t="s">
         <v>743</v>
@@ -8419,7 +7885,7 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D23" t="s">
         <v>744</v>
@@ -8433,7 +7899,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D24" t="s">
         <v>745</v>
@@ -8447,7 +7913,7 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D25" t="s">
         <v>746</v>
@@ -8461,7 +7927,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D26" t="s">
         <v>747</v>
@@ -8475,7 +7941,7 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D27" t="s">
         <v>748</v>
@@ -8489,7 +7955,7 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D28" t="s">
         <v>749</v>
@@ -8503,7 +7969,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D29" t="s">
         <v>750</v>
@@ -8517,7 +7983,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D30" t="s">
         <v>751</v>
@@ -8531,7 +7997,7 @@
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>1078</v>
+        <v>1100</v>
       </c>
       <c r="D31" t="s">
         <v>752</v>
@@ -8545,7 +8011,7 @@
         <v>720</v>
       </c>
       <c r="C32" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D32" t="s">
         <v>753</v>
@@ -8559,7 +8025,7 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D33" t="s">
         <v>754</v>
@@ -8573,7 +8039,7 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D34" t="s">
         <v>755</v>
@@ -8587,7 +8053,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D35" t="s">
         <v>756</v>
@@ -8601,7 +8067,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D36" t="s">
         <v>757</v>
@@ -8615,7 +8081,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D37" t="s">
         <v>758</v>
@@ -8629,7 +8095,7 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D38" t="s">
         <v>759</v>
@@ -8643,7 +8109,7 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D39" t="s">
         <v>760</v>
@@ -8657,7 +8123,7 @@
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D40" t="s">
         <v>761</v>
@@ -8671,7 +8137,7 @@
         <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D41" t="s">
         <v>762</v>
@@ -8685,7 +8151,7 @@
         <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D42" t="s">
         <v>763</v>
@@ -8699,7 +8165,7 @@
         <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D43" t="s">
         <v>764</v>
@@ -8713,7 +8179,7 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D44" t="s">
         <v>765</v>
@@ -8727,7 +8193,7 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D45" t="s">
         <v>766</v>
@@ -8741,7 +8207,7 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D46" t="s">
         <v>767</v>
@@ -8755,7 +8221,7 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D47" t="s">
         <v>768</v>
@@ -8769,7 +8235,7 @@
         <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D48" t="s">
         <v>769</v>
@@ -8783,7 +8249,7 @@
         <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D49" t="s">
         <v>770</v>
@@ -8797,7 +8263,7 @@
         <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D50" t="s">
         <v>771</v>
@@ -8811,7 +8277,7 @@
         <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D51" t="s">
         <v>772</v>
@@ -8825,7 +8291,7 @@
         <v>35</v>
       </c>
       <c r="C52" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D52" t="s">
         <v>773</v>
@@ -8839,7 +8305,7 @@
         <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D53" t="s">
         <v>774</v>
@@ -8853,7 +8319,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>1079</v>
+        <v>1101</v>
       </c>
       <c r="D54" t="s">
         <v>775</v>
@@ -8867,7 +8333,7 @@
         <v>720</v>
       </c>
       <c r="C55" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D55" t="s">
         <v>776</v>
@@ -8881,7 +8347,7 @@
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D56" t="s">
         <v>777</v>
@@ -8895,7 +8361,7 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D57" t="s">
         <v>778</v>
@@ -8909,7 +8375,7 @@
         <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D58" t="s">
         <v>779</v>
@@ -8923,7 +8389,7 @@
         <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D59" t="s">
         <v>780</v>
@@ -8937,7 +8403,7 @@
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D60" t="s">
         <v>781</v>
@@ -8951,7 +8417,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D61" t="s">
         <v>782</v>
@@ -8965,7 +8431,7 @@
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D62" t="s">
         <v>783</v>
@@ -8979,7 +8445,7 @@
         <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>1080</v>
+        <v>1102</v>
       </c>
       <c r="D63" t="s">
         <v>784</v>
@@ -8993,7 +8459,7 @@
         <v>720</v>
       </c>
       <c r="C64" t="s">
-        <v>1081</v>
+        <v>1103</v>
       </c>
       <c r="D64" t="s">
         <v>785</v>
@@ -9007,7 +8473,7 @@
         <v>720</v>
       </c>
       <c r="C65" t="s">
-        <v>1082</v>
+        <v>1104</v>
       </c>
       <c r="D65" t="s">
         <v>786</v>
@@ -9021,7 +8487,7 @@
         <v>720</v>
       </c>
       <c r="C66" t="s">
-        <v>1083</v>
+        <v>1105</v>
       </c>
       <c r="D66" t="s">
         <v>787</v>
@@ -9035,7 +8501,7 @@
         <v>720</v>
       </c>
       <c r="C67" t="s">
-        <v>1084</v>
+        <v>1106</v>
       </c>
       <c r="D67" t="s">
         <v>788</v>
@@ -9049,7 +8515,7 @@
         <v>720</v>
       </c>
       <c r="C68" t="s">
-        <v>1085</v>
+        <v>1107</v>
       </c>
       <c r="D68" t="s">
         <v>789</v>
@@ -9063,7 +8529,7 @@
         <v>720</v>
       </c>
       <c r="C69" t="s">
-        <v>1086</v>
+        <v>1108</v>
       </c>
       <c r="D69" t="s">
         <v>790</v>
@@ -9077,7 +8543,7 @@
         <v>720</v>
       </c>
       <c r="C70" t="s">
-        <v>1087</v>
+        <v>1109</v>
       </c>
       <c r="D70" t="s">
         <v>791</v>
@@ -9091,7 +8557,7 @@
         <v>720</v>
       </c>
       <c r="C71" t="s">
-        <v>1088</v>
+        <v>1110</v>
       </c>
       <c r="D71" t="s">
         <v>792</v>
@@ -9105,7 +8571,7 @@
         <v>720</v>
       </c>
       <c r="C72" t="s">
-        <v>1089</v>
+        <v>1111</v>
       </c>
       <c r="D72" t="s">
         <v>793</v>
@@ -9119,7 +8585,7 @@
         <v>720</v>
       </c>
       <c r="C73" t="s">
-        <v>1090</v>
+        <v>1112</v>
       </c>
       <c r="D73" t="s">
         <v>794</v>
@@ -9133,7 +8599,7 @@
         <v>720</v>
       </c>
       <c r="C74" t="s">
-        <v>1091</v>
+        <v>1113</v>
       </c>
       <c r="D74" t="s">
         <v>795</v>
@@ -9147,7 +8613,7 @@
         <v>720</v>
       </c>
       <c r="C75" t="s">
-        <v>1092</v>
+        <v>1114</v>
       </c>
       <c r="D75" t="s">
         <v>796</v>
@@ -9161,7 +8627,7 @@
         <v>720</v>
       </c>
       <c r="C76" t="s">
-        <v>1093</v>
+        <v>1115</v>
       </c>
       <c r="D76" t="s">
         <v>797</v>
@@ -9175,7 +8641,7 @@
         <v>720</v>
       </c>
       <c r="C77" t="s">
-        <v>1094</v>
+        <v>1116</v>
       </c>
       <c r="D77" t="s">
         <v>798</v>
@@ -9189,7 +8655,7 @@
         <v>720</v>
       </c>
       <c r="C78" t="s">
-        <v>1095</v>
+        <v>1117</v>
       </c>
       <c r="D78" t="s">
         <v>799</v>
@@ -9199,8 +8665,11 @@
       <c r="A79" s="20" t="s">
         <v>721</v>
       </c>
+      <c r="B79" t="s">
+        <v>720</v>
+      </c>
       <c r="C79" t="s">
-        <v>1096</v>
+        <v>1118</v>
       </c>
       <c r="D79" t="s">
         <v>800</v>
@@ -9210,8 +8679,11 @@
       <c r="A80" s="20" t="s">
         <v>722</v>
       </c>
+      <c r="B80" t="s">
+        <v>720</v>
+      </c>
       <c r="C80" t="s">
-        <v>1097</v>
+        <v>1119</v>
       </c>
       <c r="D80" t="s">
         <v>801</v>
@@ -10416,7 +9888,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>1098</v>
+        <v>1073</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>149</v>

</xml_diff>